<commit_message>
chg: upgrade trend chart maker
</commit_message>
<xml_diff>
--- a/wb.xlsx
+++ b/wb.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wryi6\Xavier_workspace\project\jzhome\JazzerLife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608580D-AE1B-4795-A1FF-475FBBFCE67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ADB3BE-1035-416E-9E35-A1D06E41518B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8DFBB6AF-22CD-4403-99A4-2591B058DECA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8DFBB6AF-22CD-4403-99A4-2591B058DECA}"/>
   </bookViews>
   <sheets>
     <sheet name=" PartsMaintenance1 " sheetId="4" r:id="rId1"/>
+    <sheet name="工作表1" sheetId="5" r:id="rId2"/>
+    <sheet name="工作表2" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">' PartsMaintenance1 '!$A$1:$K$217</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="352">
   <si>
     <t>VehicleID</t>
   </si>
@@ -1081,6 +1083,21 @@
   </si>
   <si>
     <t>https://shopee.tw/%E3%80%90D-Racing%E4%B8%89%E7%92%B0%E9%8C%B6-%E6%94%B9%E8%A3%9D%E9%8C%B6%E3%80%9160mm%E6%8C%87%E9%87%9D-%E6%95%B8%E5%AD%97%E9%9B%99%E9%A1%AF%E7%A4%BA%E7%B3%BB%E5%88%97-%E7%B5%84%E5%90%88-%E6%B0%B4%E6%BA%AB-%E6%B2%B9%E6%BA%AB-%E9%9B%BB%E5%AD%90%E5%BC%8F%E6%B2%B9%E5%A3%93%E9%8C%B6-%E6%B0%B4%E4%B8%89%E9%80%9A-%E6%A9%9F%E6%B2%B9%E8%8A%AF%E8%BD%89%E6%8E%A5%E5%BA%A7-i.42178428.5916160435</t>
+  </si>
+  <si>
+    <t>RecordID</t>
+  </si>
+  <si>
+    <t>FuelAmount</t>
+  </si>
+  <si>
+    <t>FuelCost</t>
+  </si>
+  <si>
+    <t>DistanceTravelled</t>
+  </si>
+  <si>
+    <t>FuelEfficiency</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1155,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1146,6 +1163,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1485,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67F8DA8-AA51-4542-978A-E281F3C563C4}">
   <dimension ref="A1:K217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -8148,4 +8171,2515 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8D90D8-CD60-4515-BD3D-4C881A468904}">
+  <dimension ref="A1:H93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1003</v>
+      </c>
+      <c r="B2">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C2">
+        <v>23.22</v>
+      </c>
+      <c r="D2" s="3">
+        <v>294568</v>
+      </c>
+      <c r="E2">
+        <v>13.05</v>
+      </c>
+      <c r="F2">
+        <v>303</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44972</v>
+      </c>
+      <c r="H2" s="1">
+        <v>44972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1003</v>
+      </c>
+      <c r="B3">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C3">
+        <v>32.57</v>
+      </c>
+      <c r="D3" s="3">
+        <v>294871</v>
+      </c>
+      <c r="E3">
+        <v>10.7</v>
+      </c>
+      <c r="F3">
+        <v>348</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44975</v>
+      </c>
+      <c r="H3" s="1">
+        <v>44975</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4">
+        <v>32.6</v>
+      </c>
+      <c r="C4">
+        <v>33.99</v>
+      </c>
+      <c r="D4" s="3">
+        <v>295219</v>
+      </c>
+      <c r="E4">
+        <v>7.1</v>
+      </c>
+      <c r="F4">
+        <v>242</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44978</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44978</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5">
+        <v>32.5</v>
+      </c>
+      <c r="C5">
+        <v>23.2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>295461</v>
+      </c>
+      <c r="E5">
+        <v>11.6</v>
+      </c>
+      <c r="F5">
+        <v>270</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44985</v>
+      </c>
+      <c r="H5" s="1">
+        <v>44985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1003</v>
+      </c>
+      <c r="B6">
+        <v>32.4</v>
+      </c>
+      <c r="C6">
+        <v>24.37</v>
+      </c>
+      <c r="D6" s="3">
+        <v>295731</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>267</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44986</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1003</v>
+      </c>
+      <c r="B7">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C7">
+        <v>38.049999999999997</v>
+      </c>
+      <c r="D7" s="3">
+        <v>295998</v>
+      </c>
+      <c r="E7">
+        <v>13.7</v>
+      </c>
+      <c r="F7">
+        <v>522</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44997</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1003</v>
+      </c>
+      <c r="B8">
+        <v>31.9</v>
+      </c>
+      <c r="C8">
+        <v>35.32</v>
+      </c>
+      <c r="D8" s="3">
+        <v>296520</v>
+      </c>
+      <c r="E8">
+        <v>10.6</v>
+      </c>
+      <c r="F8">
+        <v>374</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45018</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1003</v>
+      </c>
+      <c r="B9">
+        <v>32.4</v>
+      </c>
+      <c r="C9">
+        <v>20.99</v>
+      </c>
+      <c r="D9" s="3">
+        <v>297360</v>
+      </c>
+      <c r="E9">
+        <v>11.9</v>
+      </c>
+      <c r="F9">
+        <v>250</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45019</v>
+      </c>
+      <c r="H9" s="1">
+        <v>45019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1003</v>
+      </c>
+      <c r="B10">
+        <v>32.4</v>
+      </c>
+      <c r="C10">
+        <v>29.69</v>
+      </c>
+      <c r="D10" s="3">
+        <v>297681</v>
+      </c>
+      <c r="E10">
+        <v>10.8</v>
+      </c>
+      <c r="F10">
+        <v>321</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45025</v>
+      </c>
+      <c r="H10" s="1">
+        <v>45025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1003</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>35.28</v>
+      </c>
+      <c r="D11" s="3">
+        <v>298203</v>
+      </c>
+      <c r="E11">
+        <v>14.8</v>
+      </c>
+      <c r="F11">
+        <v>522</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45026</v>
+      </c>
+      <c r="H11" s="1">
+        <v>45026</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1003</v>
+      </c>
+      <c r="B12">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>29.45</v>
+      </c>
+      <c r="D12" s="3">
+        <v>298638</v>
+      </c>
+      <c r="E12">
+        <v>14.8</v>
+      </c>
+      <c r="F12">
+        <v>435</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45047</v>
+      </c>
+      <c r="H12" s="1">
+        <v>45047</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1003</v>
+      </c>
+      <c r="B13">
+        <v>32.4</v>
+      </c>
+      <c r="C13">
+        <v>6.3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>298711</v>
+      </c>
+      <c r="E13">
+        <v>11.6</v>
+      </c>
+      <c r="F13">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45076</v>
+      </c>
+      <c r="H13" s="1">
+        <v>45076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1003</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>25.49</v>
+      </c>
+      <c r="D14">
+        <v>298962</v>
+      </c>
+      <c r="E14">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F14">
+        <v>251</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45102</v>
+      </c>
+      <c r="H14" s="1">
+        <v>45102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1003</v>
+      </c>
+      <c r="B15">
+        <v>30.6</v>
+      </c>
+      <c r="C15">
+        <v>35.24</v>
+      </c>
+      <c r="D15">
+        <v>299503</v>
+      </c>
+      <c r="E15">
+        <v>15.4</v>
+      </c>
+      <c r="F15">
+        <v>541</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45117</v>
+      </c>
+      <c r="H15" s="1">
+        <v>45117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1003</v>
+      </c>
+      <c r="B16">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C16">
+        <v>37.58</v>
+      </c>
+      <c r="D16">
+        <v>300163</v>
+      </c>
+      <c r="E16">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F16">
+        <v>660</v>
+      </c>
+      <c r="G16" s="1">
+        <v>45130</v>
+      </c>
+      <c r="H16" s="1">
+        <v>45130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1003</v>
+      </c>
+      <c r="B17">
+        <v>34.6</v>
+      </c>
+      <c r="C17">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>300807</v>
+      </c>
+      <c r="E17">
+        <v>20.8</v>
+      </c>
+      <c r="F17">
+        <v>644</v>
+      </c>
+      <c r="G17" s="1">
+        <v>45156</v>
+      </c>
+      <c r="H17" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1003</v>
+      </c>
+      <c r="B18">
+        <v>34.6</v>
+      </c>
+      <c r="C18">
+        <v>30.63</v>
+      </c>
+      <c r="D18">
+        <v>301146</v>
+      </c>
+      <c r="E18">
+        <v>11.1</v>
+      </c>
+      <c r="F18">
+        <v>339</v>
+      </c>
+      <c r="G18" s="1">
+        <v>45164</v>
+      </c>
+      <c r="H18" s="1">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1003</v>
+      </c>
+      <c r="B19">
+        <v>34.6</v>
+      </c>
+      <c r="C19">
+        <v>25.803000000000001</v>
+      </c>
+      <c r="D19">
+        <v>301469</v>
+      </c>
+      <c r="E19">
+        <v>12.5</v>
+      </c>
+      <c r="F19">
+        <v>323</v>
+      </c>
+      <c r="G19" s="1">
+        <v>45165</v>
+      </c>
+      <c r="H19" s="1">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1003</v>
+      </c>
+      <c r="B20">
+        <v>35.1</v>
+      </c>
+      <c r="C20">
+        <v>24.27</v>
+      </c>
+      <c r="D20">
+        <v>301647</v>
+      </c>
+      <c r="E20">
+        <v>7.3</v>
+      </c>
+      <c r="F20">
+        <v>178</v>
+      </c>
+      <c r="G20" s="1">
+        <v>45185</v>
+      </c>
+      <c r="H20" s="1">
+        <v>45185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1003</v>
+      </c>
+      <c r="B21">
+        <v>34.9</v>
+      </c>
+      <c r="C21">
+        <v>29.63</v>
+      </c>
+      <c r="D21">
+        <v>301956</v>
+      </c>
+      <c r="E21">
+        <v>10.4</v>
+      </c>
+      <c r="F21">
+        <v>309</v>
+      </c>
+      <c r="G21" s="1">
+        <v>45192</v>
+      </c>
+      <c r="H21" s="1">
+        <v>45192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1003</v>
+      </c>
+      <c r="B22">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="C22">
+        <v>27.08</v>
+      </c>
+      <c r="D22">
+        <v>302261</v>
+      </c>
+      <c r="E22">
+        <v>11.3</v>
+      </c>
+      <c r="F22">
+        <v>305</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45207</v>
+      </c>
+      <c r="H22" s="1">
+        <v>45207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1003</v>
+      </c>
+      <c r="B23">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="C23">
+        <v>20.56</v>
+      </c>
+      <c r="D23">
+        <v>302459</v>
+      </c>
+      <c r="E23">
+        <v>9.6</v>
+      </c>
+      <c r="F23">
+        <v>198</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45214</v>
+      </c>
+      <c r="H23" s="1">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1003</v>
+      </c>
+      <c r="B24">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C24">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="D24">
+        <v>302705</v>
+      </c>
+      <c r="E24">
+        <v>12.1</v>
+      </c>
+      <c r="F24">
+        <v>246</v>
+      </c>
+      <c r="G24" s="1">
+        <v>45216</v>
+      </c>
+      <c r="H24" s="1">
+        <v>45216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1003</v>
+      </c>
+      <c r="B25">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="C25">
+        <v>27.76</v>
+      </c>
+      <c r="D25">
+        <v>303017</v>
+      </c>
+      <c r="E25">
+        <v>11.2</v>
+      </c>
+      <c r="F25">
+        <v>312</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45221</v>
+      </c>
+      <c r="H25" s="1">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1003</v>
+      </c>
+      <c r="B26">
+        <v>33.4</v>
+      </c>
+      <c r="C26">
+        <v>30.7</v>
+      </c>
+      <c r="D26">
+        <v>303381</v>
+      </c>
+      <c r="E26">
+        <v>11.9</v>
+      </c>
+      <c r="F26">
+        <v>364</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45226</v>
+      </c>
+      <c r="H26" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1003</v>
+      </c>
+      <c r="B27">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C27">
+        <v>29.57</v>
+      </c>
+      <c r="D27">
+        <v>303762</v>
+      </c>
+      <c r="E27">
+        <v>12.9</v>
+      </c>
+      <c r="F27">
+        <v>381</v>
+      </c>
+      <c r="G27" s="1">
+        <v>45236</v>
+      </c>
+      <c r="H27" s="1">
+        <v>45236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1003</v>
+      </c>
+      <c r="B28">
+        <v>33.1</v>
+      </c>
+      <c r="C28">
+        <v>25.7</v>
+      </c>
+      <c r="D28">
+        <v>304004</v>
+      </c>
+      <c r="E28">
+        <v>9.4</v>
+      </c>
+      <c r="F28">
+        <v>242</v>
+      </c>
+      <c r="G28" s="1">
+        <v>45246</v>
+      </c>
+      <c r="H28" s="1">
+        <v>45246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1003</v>
+      </c>
+      <c r="B29">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C29">
+        <v>29.83</v>
+      </c>
+      <c r="D29">
+        <v>304469</v>
+      </c>
+      <c r="E29">
+        <v>15.6</v>
+      </c>
+      <c r="F29">
+        <v>465</v>
+      </c>
+      <c r="G29" s="1">
+        <v>45283</v>
+      </c>
+      <c r="H29" s="1">
+        <v>45283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1003</v>
+      </c>
+      <c r="B30">
+        <v>33.1</v>
+      </c>
+      <c r="C30">
+        <v>26.649000000000001</v>
+      </c>
+      <c r="D30">
+        <v>305015</v>
+      </c>
+      <c r="E30">
+        <v>20.5</v>
+      </c>
+      <c r="F30">
+        <v>546</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45290</v>
+      </c>
+      <c r="H30" s="1">
+        <v>45290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1003</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>35</v>
+      </c>
+      <c r="D31">
+        <v>305426</v>
+      </c>
+      <c r="E31">
+        <v>11.7</v>
+      </c>
+      <c r="F31">
+        <v>411</v>
+      </c>
+      <c r="G31" s="1">
+        <v>45292</v>
+      </c>
+      <c r="H31" s="1">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1003</v>
+      </c>
+      <c r="B32">
+        <v>32.4</v>
+      </c>
+      <c r="C32">
+        <v>25.49</v>
+      </c>
+      <c r="D32">
+        <v>305701</v>
+      </c>
+      <c r="E32">
+        <v>10.8</v>
+      </c>
+      <c r="F32">
+        <v>275</v>
+      </c>
+      <c r="G32" s="1">
+        <v>45317</v>
+      </c>
+      <c r="H32" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1003</v>
+      </c>
+      <c r="B33">
+        <v>32.4</v>
+      </c>
+      <c r="C33">
+        <v>30.242999999999999</v>
+      </c>
+      <c r="D33">
+        <v>306001</v>
+      </c>
+      <c r="E33">
+        <v>9.9</v>
+      </c>
+      <c r="F33">
+        <v>300</v>
+      </c>
+      <c r="G33" s="1">
+        <v>45326</v>
+      </c>
+      <c r="H33" s="1">
+        <v>45326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1003</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>29.15</v>
+      </c>
+      <c r="D34">
+        <v>306291</v>
+      </c>
+      <c r="E34">
+        <v>9.9</v>
+      </c>
+      <c r="F34">
+        <v>290</v>
+      </c>
+      <c r="G34" s="1">
+        <v>45368</v>
+      </c>
+      <c r="H34" s="1">
+        <v>45368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1003</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>29.821000000000002</v>
+      </c>
+      <c r="D35">
+        <v>306650</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>359</v>
+      </c>
+      <c r="G35" s="1">
+        <v>45382</v>
+      </c>
+      <c r="H35" s="1">
+        <v>45382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1003</v>
+      </c>
+      <c r="B36">
+        <v>33.1</v>
+      </c>
+      <c r="C36">
+        <v>27.733000000000001</v>
+      </c>
+      <c r="D36">
+        <v>306919</v>
+      </c>
+      <c r="E36">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F36">
+        <v>269</v>
+      </c>
+      <c r="G36" s="1">
+        <v>45399</v>
+      </c>
+      <c r="H36" s="1">
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1003</v>
+      </c>
+      <c r="B37">
+        <v>32.9</v>
+      </c>
+      <c r="C37">
+        <v>30.1</v>
+      </c>
+      <c r="D37">
+        <v>307356</v>
+      </c>
+      <c r="E37">
+        <v>14.5</v>
+      </c>
+      <c r="F37">
+        <v>437</v>
+      </c>
+      <c r="G37" s="1">
+        <v>45420</v>
+      </c>
+      <c r="H37" s="1">
+        <v>45420</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1003</v>
+      </c>
+      <c r="B38">
+        <v>32.9</v>
+      </c>
+      <c r="C38">
+        <v>27.89</v>
+      </c>
+      <c r="D38">
+        <v>307670</v>
+      </c>
+      <c r="E38">
+        <v>11.3</v>
+      </c>
+      <c r="F38">
+        <v>314</v>
+      </c>
+      <c r="G38" s="1">
+        <v>45426</v>
+      </c>
+      <c r="H38" s="1">
+        <v>45426</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1003</v>
+      </c>
+      <c r="B39">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C39">
+        <v>29.35</v>
+      </c>
+      <c r="D39">
+        <v>308070</v>
+      </c>
+      <c r="E39">
+        <v>13.6</v>
+      </c>
+      <c r="F39">
+        <v>400</v>
+      </c>
+      <c r="G39" s="1">
+        <v>45440</v>
+      </c>
+      <c r="H39" s="1">
+        <v>45440</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1003</v>
+      </c>
+      <c r="B40">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C40">
+        <v>26.71</v>
+      </c>
+      <c r="D40">
+        <v>308314</v>
+      </c>
+      <c r="E40">
+        <v>9.1</v>
+      </c>
+      <c r="F40">
+        <v>244</v>
+      </c>
+      <c r="G40" s="1">
+        <v>45444</v>
+      </c>
+      <c r="H40" s="1">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1003</v>
+      </c>
+      <c r="B41">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C41">
+        <v>22.7</v>
+      </c>
+      <c r="D41">
+        <v>308543</v>
+      </c>
+      <c r="E41">
+        <v>10.1</v>
+      </c>
+      <c r="F41">
+        <v>229</v>
+      </c>
+      <c r="G41" s="1">
+        <v>45450</v>
+      </c>
+      <c r="H41" s="1">
+        <v>45450</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1003</v>
+      </c>
+      <c r="B42">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C42">
+        <v>30.43</v>
+      </c>
+      <c r="D42">
+        <v>308850</v>
+      </c>
+      <c r="E42">
+        <v>10.1</v>
+      </c>
+      <c r="F42">
+        <v>307</v>
+      </c>
+      <c r="G42" s="1">
+        <v>45460</v>
+      </c>
+      <c r="H42" s="1">
+        <v>45460</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1003</v>
+      </c>
+      <c r="B43">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C43">
+        <v>27.65</v>
+      </c>
+      <c r="D43">
+        <v>309205</v>
+      </c>
+      <c r="E43">
+        <v>12.8</v>
+      </c>
+      <c r="F43">
+        <v>355</v>
+      </c>
+      <c r="G43" s="1">
+        <v>45464</v>
+      </c>
+      <c r="H43" s="1">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1003</v>
+      </c>
+      <c r="B44">
+        <v>32.4</v>
+      </c>
+      <c r="C44">
+        <v>24.04</v>
+      </c>
+      <c r="D44">
+        <v>309413</v>
+      </c>
+      <c r="E44">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F44">
+        <v>208</v>
+      </c>
+      <c r="G44" s="1">
+        <v>45477</v>
+      </c>
+      <c r="H44" s="1">
+        <v>45477</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1003</v>
+      </c>
+      <c r="B45">
+        <v>32.4</v>
+      </c>
+      <c r="C45">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="D45">
+        <v>309804</v>
+      </c>
+      <c r="E45">
+        <v>11.5</v>
+      </c>
+      <c r="F45">
+        <v>391</v>
+      </c>
+      <c r="G45" s="1">
+        <v>45479</v>
+      </c>
+      <c r="H45" s="1">
+        <v>45479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1003</v>
+      </c>
+      <c r="B46">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C46">
+        <v>32.159999999999997</v>
+      </c>
+      <c r="D46">
+        <v>310139</v>
+      </c>
+      <c r="E46">
+        <v>10.4</v>
+      </c>
+      <c r="F46">
+        <v>335</v>
+      </c>
+      <c r="G46" s="1">
+        <v>45501</v>
+      </c>
+      <c r="H46" s="1">
+        <v>45501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1003</v>
+      </c>
+      <c r="B47">
+        <v>33.6</v>
+      </c>
+      <c r="C47">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="D47">
+        <v>310447</v>
+      </c>
+      <c r="E47">
+        <v>9</v>
+      </c>
+      <c r="F47">
+        <v>308</v>
+      </c>
+      <c r="G47" s="1">
+        <v>45523</v>
+      </c>
+      <c r="H47" s="1">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1003</v>
+      </c>
+      <c r="B48">
+        <v>33.4</v>
+      </c>
+      <c r="C48">
+        <v>30.03</v>
+      </c>
+      <c r="D48">
+        <v>310787</v>
+      </c>
+      <c r="E48">
+        <v>11.3</v>
+      </c>
+      <c r="F48">
+        <v>340</v>
+      </c>
+      <c r="G48" s="1">
+        <v>45530</v>
+      </c>
+      <c r="H48" s="1">
+        <v>45530</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1003</v>
+      </c>
+      <c r="B49">
+        <v>33.4</v>
+      </c>
+      <c r="C49">
+        <v>28.42</v>
+      </c>
+      <c r="D49">
+        <v>311106</v>
+      </c>
+      <c r="E49">
+        <v>11.2</v>
+      </c>
+      <c r="F49">
+        <v>319</v>
+      </c>
+      <c r="G49" s="1">
+        <v>45534</v>
+      </c>
+      <c r="H49" s="1">
+        <v>45534</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1003</v>
+      </c>
+      <c r="B50">
+        <v>33.4</v>
+      </c>
+      <c r="C50">
+        <v>15.03</v>
+      </c>
+      <c r="D50">
+        <v>311275</v>
+      </c>
+      <c r="E50">
+        <v>11.2</v>
+      </c>
+      <c r="F50">
+        <v>169</v>
+      </c>
+      <c r="G50" s="1">
+        <v>45535</v>
+      </c>
+      <c r="H50" s="1">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1003</v>
+      </c>
+      <c r="B51">
+        <v>33.6</v>
+      </c>
+      <c r="C51">
+        <v>20.75</v>
+      </c>
+      <c r="D51">
+        <v>311491</v>
+      </c>
+      <c r="E51">
+        <v>10.4</v>
+      </c>
+      <c r="F51">
+        <v>216</v>
+      </c>
+      <c r="G51" s="1">
+        <v>45541</v>
+      </c>
+      <c r="H51" s="1">
+        <v>45541</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1003</v>
+      </c>
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <v>23.13</v>
+      </c>
+      <c r="D52">
+        <v>311711</v>
+      </c>
+      <c r="E52">
+        <v>9.5</v>
+      </c>
+      <c r="F52">
+        <v>220</v>
+      </c>
+      <c r="G52" s="1">
+        <v>45543</v>
+      </c>
+      <c r="H52" s="1">
+        <v>45543</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1003</v>
+      </c>
+      <c r="B53">
+        <v>32.5</v>
+      </c>
+      <c r="C53">
+        <v>28.16</v>
+      </c>
+      <c r="D53">
+        <v>312015</v>
+      </c>
+      <c r="E53">
+        <v>10.8</v>
+      </c>
+      <c r="F53">
+        <v>304</v>
+      </c>
+      <c r="G53" s="1">
+        <v>45550</v>
+      </c>
+      <c r="H53" s="1">
+        <v>45550</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1003</v>
+      </c>
+      <c r="B54">
+        <v>32.5</v>
+      </c>
+      <c r="C54">
+        <v>159.72200000000001</v>
+      </c>
+      <c r="D54">
+        <v>313740</v>
+      </c>
+      <c r="E54">
+        <v>10.8</v>
+      </c>
+      <c r="F54">
+        <v>1725</v>
+      </c>
+      <c r="G54" s="1">
+        <v>45576</v>
+      </c>
+      <c r="H54" s="1">
+        <v>45576</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1003</v>
+      </c>
+      <c r="B55">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C55">
+        <v>30.71</v>
+      </c>
+      <c r="D55">
+        <v>314540</v>
+      </c>
+      <c r="E55">
+        <v>10.8</v>
+      </c>
+      <c r="F55">
+        <v>800</v>
+      </c>
+      <c r="G55" s="1">
+        <v>45588</v>
+      </c>
+      <c r="H55" s="1">
+        <v>45588</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1003</v>
+      </c>
+      <c r="B56">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C56">
+        <v>28.68</v>
+      </c>
+      <c r="D56">
+        <v>315241</v>
+      </c>
+      <c r="E56">
+        <v>10.8</v>
+      </c>
+      <c r="F56">
+        <v>701</v>
+      </c>
+      <c r="G56" s="1">
+        <v>45601</v>
+      </c>
+      <c r="H56" s="1">
+        <v>45601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1003</v>
+      </c>
+      <c r="B57">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C57">
+        <v>22.91</v>
+      </c>
+      <c r="D57">
+        <v>315501</v>
+      </c>
+      <c r="E57">
+        <v>11.3</v>
+      </c>
+      <c r="F57">
+        <v>260</v>
+      </c>
+      <c r="G57" s="1">
+        <v>45605</v>
+      </c>
+      <c r="H57" s="1">
+        <v>45605</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1003</v>
+      </c>
+      <c r="B58">
+        <v>32.1</v>
+      </c>
+      <c r="C58">
+        <v>34.340000000000003</v>
+      </c>
+      <c r="D58">
+        <v>316684</v>
+      </c>
+      <c r="E58">
+        <v>11.3</v>
+      </c>
+      <c r="F58">
+        <v>1183</v>
+      </c>
+      <c r="G58" s="1">
+        <v>45616</v>
+      </c>
+      <c r="H58" s="1">
+        <v>45616</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1003</v>
+      </c>
+      <c r="B59">
+        <v>32.1</v>
+      </c>
+      <c r="C59">
+        <v>27.06</v>
+      </c>
+      <c r="D59">
+        <v>317031</v>
+      </c>
+      <c r="E59">
+        <v>12.8</v>
+      </c>
+      <c r="F59">
+        <v>347</v>
+      </c>
+      <c r="G59" s="1">
+        <v>45619</v>
+      </c>
+      <c r="H59" s="1">
+        <v>45619</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1003</v>
+      </c>
+      <c r="B60">
+        <v>32.1</v>
+      </c>
+      <c r="C60">
+        <v>30.64</v>
+      </c>
+      <c r="D60">
+        <v>317384</v>
+      </c>
+      <c r="E60">
+        <v>11.5</v>
+      </c>
+      <c r="F60">
+        <v>353</v>
+      </c>
+      <c r="G60" s="1">
+        <v>45623</v>
+      </c>
+      <c r="H60" s="1">
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1003</v>
+      </c>
+      <c r="B61">
+        <v>32.1</v>
+      </c>
+      <c r="C61">
+        <v>38.89</v>
+      </c>
+      <c r="D61">
+        <v>318113</v>
+      </c>
+      <c r="E61">
+        <v>11.5</v>
+      </c>
+      <c r="F61">
+        <v>729</v>
+      </c>
+      <c r="G61" s="1">
+        <v>45626</v>
+      </c>
+      <c r="H61" s="1">
+        <v>45626</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1003</v>
+      </c>
+      <c r="B62">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C62">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D62">
+        <v>318368</v>
+      </c>
+      <c r="E62">
+        <v>13.4</v>
+      </c>
+      <c r="F62">
+        <v>255</v>
+      </c>
+      <c r="G62" s="1">
+        <v>45630</v>
+      </c>
+      <c r="H62" s="1">
+        <v>45630</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1003</v>
+      </c>
+      <c r="B63">
+        <v>32.1</v>
+      </c>
+      <c r="C63">
+        <v>25.74</v>
+      </c>
+      <c r="D63">
+        <v>318645</v>
+      </c>
+      <c r="E63">
+        <v>10.8</v>
+      </c>
+      <c r="F63">
+        <v>277</v>
+      </c>
+      <c r="G63" s="1">
+        <v>45639</v>
+      </c>
+      <c r="H63" s="1">
+        <v>45639</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1003</v>
+      </c>
+      <c r="B64">
+        <v>32.1</v>
+      </c>
+      <c r="C64">
+        <v>31.59</v>
+      </c>
+      <c r="D64">
+        <v>319011</v>
+      </c>
+      <c r="E64">
+        <v>11.6</v>
+      </c>
+      <c r="F64">
+        <v>366</v>
+      </c>
+      <c r="G64" s="1">
+        <v>45640</v>
+      </c>
+      <c r="H64" s="1">
+        <v>45640</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1003</v>
+      </c>
+      <c r="B65">
+        <v>32</v>
+      </c>
+      <c r="C65">
+        <v>42.16</v>
+      </c>
+      <c r="D65">
+        <v>319584</v>
+      </c>
+      <c r="E65">
+        <v>13.6</v>
+      </c>
+      <c r="F65">
+        <v>573</v>
+      </c>
+      <c r="G65" s="1">
+        <v>45642</v>
+      </c>
+      <c r="H65" s="1">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1003</v>
+      </c>
+      <c r="B66">
+        <v>32</v>
+      </c>
+      <c r="C66">
+        <v>39.78125</v>
+      </c>
+      <c r="D66">
+        <v>320025</v>
+      </c>
+      <c r="E66">
+        <v>11.1</v>
+      </c>
+      <c r="F66">
+        <v>441</v>
+      </c>
+      <c r="G66" s="1">
+        <v>45649</v>
+      </c>
+      <c r="H66" s="1">
+        <v>45649</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1003</v>
+      </c>
+      <c r="B67">
+        <v>32.1</v>
+      </c>
+      <c r="C67">
+        <v>28.6</v>
+      </c>
+      <c r="D67">
+        <v>320306</v>
+      </c>
+      <c r="E67">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F67">
+        <v>281</v>
+      </c>
+      <c r="G67" s="1">
+        <v>45653</v>
+      </c>
+      <c r="H67" s="1">
+        <v>45653</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1003</v>
+      </c>
+      <c r="B68">
+        <v>32.1</v>
+      </c>
+      <c r="C68">
+        <v>125</v>
+      </c>
+      <c r="D68">
+        <v>321580</v>
+      </c>
+      <c r="E68">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F68">
+        <v>1274</v>
+      </c>
+      <c r="G68" s="1">
+        <v>45665</v>
+      </c>
+      <c r="H68" s="1">
+        <v>45665</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1003</v>
+      </c>
+      <c r="B69">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C69">
+        <v>30.57</v>
+      </c>
+      <c r="D69">
+        <v>322301</v>
+      </c>
+      <c r="E69">
+        <v>23.6</v>
+      </c>
+      <c r="F69">
+        <v>721</v>
+      </c>
+      <c r="G69" s="1">
+        <v>45671</v>
+      </c>
+      <c r="H69" s="1">
+        <v>45671</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1003</v>
+      </c>
+      <c r="B70">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C70">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="D70">
+        <v>322680</v>
+      </c>
+      <c r="E70">
+        <v>11</v>
+      </c>
+      <c r="F70">
+        <v>379</v>
+      </c>
+      <c r="G70" s="1">
+        <v>45676</v>
+      </c>
+      <c r="H70" s="1">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1003</v>
+      </c>
+      <c r="B71">
+        <v>33.1</v>
+      </c>
+      <c r="C71">
+        <v>28.82</v>
+      </c>
+      <c r="D71">
+        <v>323061</v>
+      </c>
+      <c r="E71">
+        <v>13.2</v>
+      </c>
+      <c r="F71">
+        <v>381</v>
+      </c>
+      <c r="G71" s="1">
+        <v>45682</v>
+      </c>
+      <c r="H71" s="1">
+        <v>45682</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1003</v>
+      </c>
+      <c r="B72">
+        <v>33.1</v>
+      </c>
+      <c r="C72">
+        <v>30.76</v>
+      </c>
+      <c r="D72">
+        <v>323431</v>
+      </c>
+      <c r="E72">
+        <v>12</v>
+      </c>
+      <c r="F72">
+        <v>370</v>
+      </c>
+      <c r="G72" s="1">
+        <v>45686</v>
+      </c>
+      <c r="H72" s="1">
+        <v>45686</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1003</v>
+      </c>
+      <c r="B73">
+        <v>33.1</v>
+      </c>
+      <c r="C73">
+        <v>18.87</v>
+      </c>
+      <c r="D73">
+        <v>323706</v>
+      </c>
+      <c r="E73">
+        <v>14.6</v>
+      </c>
+      <c r="F73">
+        <v>275</v>
+      </c>
+      <c r="G73" s="1">
+        <v>45687</v>
+      </c>
+      <c r="H73" s="1">
+        <v>45687</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1003</v>
+      </c>
+      <c r="B74">
+        <v>33.1</v>
+      </c>
+      <c r="C74">
+        <v>22.32</v>
+      </c>
+      <c r="D74">
+        <v>324002</v>
+      </c>
+      <c r="E74">
+        <v>13.3</v>
+      </c>
+      <c r="F74">
+        <v>296</v>
+      </c>
+      <c r="G74" s="1">
+        <v>45689</v>
+      </c>
+      <c r="H74" s="1">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1003</v>
+      </c>
+      <c r="B75">
+        <v>33.1</v>
+      </c>
+      <c r="C75">
+        <v>27.74</v>
+      </c>
+      <c r="D75">
+        <v>324377</v>
+      </c>
+      <c r="E75">
+        <v>13.5</v>
+      </c>
+      <c r="F75">
+        <v>375</v>
+      </c>
+      <c r="G75" s="1">
+        <v>45691</v>
+      </c>
+      <c r="H75" s="1">
+        <v>45691</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1003</v>
+      </c>
+      <c r="B76">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C76">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="D76">
+        <v>325777</v>
+      </c>
+      <c r="E76">
+        <v>38.6</v>
+      </c>
+      <c r="F76">
+        <v>1400</v>
+      </c>
+      <c r="G76" s="1">
+        <v>45712</v>
+      </c>
+      <c r="H76" s="1">
+        <v>45712</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1003</v>
+      </c>
+      <c r="B77">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C77">
+        <v>38.520000000000003</v>
+      </c>
+      <c r="D77">
+        <v>326246</v>
+      </c>
+      <c r="E77">
+        <v>12.2</v>
+      </c>
+      <c r="F77">
+        <v>469</v>
+      </c>
+      <c r="G77" s="1">
+        <v>45718</v>
+      </c>
+      <c r="H77" s="1">
+        <v>45718</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1003</v>
+      </c>
+      <c r="B78">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="C78">
+        <v>27.82</v>
+      </c>
+      <c r="D78">
+        <v>326625</v>
+      </c>
+      <c r="E78">
+        <v>13.6</v>
+      </c>
+      <c r="F78">
+        <v>379</v>
+      </c>
+      <c r="G78" s="1">
+        <v>45723</v>
+      </c>
+      <c r="H78" s="1">
+        <v>45723</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1003</v>
+      </c>
+      <c r="B79">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C79">
+        <v>34.83</v>
+      </c>
+      <c r="D79">
+        <v>326977</v>
+      </c>
+      <c r="E79">
+        <v>10.1</v>
+      </c>
+      <c r="F79">
+        <v>352</v>
+      </c>
+      <c r="G79" s="1">
+        <v>45727</v>
+      </c>
+      <c r="H79" s="1">
+        <v>45727</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1003</v>
+      </c>
+      <c r="B80">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C80">
+        <v>31.84</v>
+      </c>
+      <c r="D80">
+        <v>327373</v>
+      </c>
+      <c r="E80">
+        <v>12.4</v>
+      </c>
+      <c r="F80">
+        <v>396</v>
+      </c>
+      <c r="G80" s="1">
+        <v>45731</v>
+      </c>
+      <c r="H80" s="1">
+        <v>45731</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1003</v>
+      </c>
+      <c r="B81">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C81">
+        <v>36.99</v>
+      </c>
+      <c r="D81">
+        <v>327797</v>
+      </c>
+      <c r="E81">
+        <v>12.4</v>
+      </c>
+      <c r="F81">
+        <v>396</v>
+      </c>
+      <c r="G81" s="1">
+        <v>45735</v>
+      </c>
+      <c r="H81" s="1">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1003</v>
+      </c>
+      <c r="B82">
+        <v>32.4</v>
+      </c>
+      <c r="C82">
+        <v>31.91</v>
+      </c>
+      <c r="D82">
+        <v>328181</v>
+      </c>
+      <c r="E82">
+        <v>12</v>
+      </c>
+      <c r="F82">
+        <v>384</v>
+      </c>
+      <c r="G82" s="1">
+        <v>45740</v>
+      </c>
+      <c r="H82" s="1">
+        <v>45740</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1003</v>
+      </c>
+      <c r="B83">
+        <v>32.4</v>
+      </c>
+      <c r="C83">
+        <v>23.51</v>
+      </c>
+      <c r="D83">
+        <v>328464</v>
+      </c>
+      <c r="E83">
+        <v>12</v>
+      </c>
+      <c r="F83">
+        <v>283</v>
+      </c>
+      <c r="G83" s="1">
+        <v>45743</v>
+      </c>
+      <c r="H83" s="1">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1003</v>
+      </c>
+      <c r="B84">
+        <v>32.4</v>
+      </c>
+      <c r="C84">
+        <v>35.51</v>
+      </c>
+      <c r="D84">
+        <v>328868</v>
+      </c>
+      <c r="E84">
+        <v>11.4</v>
+      </c>
+      <c r="F84">
+        <v>404</v>
+      </c>
+      <c r="G84" s="1">
+        <v>45746</v>
+      </c>
+      <c r="H84" s="1">
+        <v>45746</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1003</v>
+      </c>
+      <c r="B85">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C85">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="D85">
+        <v>329282</v>
+      </c>
+      <c r="E85">
+        <v>12.5</v>
+      </c>
+      <c r="F85">
+        <v>414</v>
+      </c>
+      <c r="G85" s="1">
+        <v>45749</v>
+      </c>
+      <c r="H85" s="1">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1003</v>
+      </c>
+      <c r="B86">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C86">
+        <v>25.42</v>
+      </c>
+      <c r="D86">
+        <v>329599</v>
+      </c>
+      <c r="E86">
+        <v>12.5</v>
+      </c>
+      <c r="F86">
+        <v>317</v>
+      </c>
+      <c r="G86" s="1">
+        <v>45752</v>
+      </c>
+      <c r="H86" s="1">
+        <v>45752</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1003</v>
+      </c>
+      <c r="B87">
+        <v>32.1</v>
+      </c>
+      <c r="C87">
+        <v>31.75</v>
+      </c>
+      <c r="D87">
+        <v>329971</v>
+      </c>
+      <c r="E87">
+        <v>11.7</v>
+      </c>
+      <c r="F87">
+        <v>372</v>
+      </c>
+      <c r="G87" s="1">
+        <v>45754</v>
+      </c>
+      <c r="H87" s="1">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1003</v>
+      </c>
+      <c r="B88">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="C88">
+        <v>32.4</v>
+      </c>
+      <c r="D88">
+        <v>330390</v>
+      </c>
+      <c r="E88">
+        <v>12.9</v>
+      </c>
+      <c r="F88">
+        <v>419</v>
+      </c>
+      <c r="G88" s="1">
+        <v>45759</v>
+      </c>
+      <c r="H88" s="1">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1003</v>
+      </c>
+      <c r="B89">
+        <v>31.4</v>
+      </c>
+      <c r="C89">
+        <v>32.61</v>
+      </c>
+      <c r="D89">
+        <v>330751</v>
+      </c>
+      <c r="E89">
+        <v>11.1</v>
+      </c>
+      <c r="F89">
+        <v>361</v>
+      </c>
+      <c r="G89" s="1">
+        <v>45766</v>
+      </c>
+      <c r="H89" s="1">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1003</v>
+      </c>
+      <c r="B90">
+        <v>31.8</v>
+      </c>
+      <c r="C90">
+        <v>31.43</v>
+      </c>
+      <c r="D90">
+        <v>331139</v>
+      </c>
+      <c r="E90">
+        <v>12.3</v>
+      </c>
+      <c r="F90">
+        <v>388</v>
+      </c>
+      <c r="G90" s="1">
+        <v>45767</v>
+      </c>
+      <c r="H90" s="1">
+        <v>45767</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1003</v>
+      </c>
+      <c r="B91">
+        <v>31.8</v>
+      </c>
+      <c r="C91">
+        <v>32.01</v>
+      </c>
+      <c r="D91">
+        <v>331530</v>
+      </c>
+      <c r="E91">
+        <v>12.2</v>
+      </c>
+      <c r="F91">
+        <v>391</v>
+      </c>
+      <c r="G91" s="1">
+        <v>45772</v>
+      </c>
+      <c r="H91" s="1">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1003</v>
+      </c>
+      <c r="B92">
+        <v>31.8</v>
+      </c>
+      <c r="C92">
+        <v>26.97</v>
+      </c>
+      <c r="D92">
+        <v>331830</v>
+      </c>
+      <c r="E92">
+        <v>11.1</v>
+      </c>
+      <c r="F92">
+        <v>300</v>
+      </c>
+      <c r="G92" s="1">
+        <v>45775</v>
+      </c>
+      <c r="H92" s="1">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1003</v>
+      </c>
+      <c r="B93">
+        <v>31.8</v>
+      </c>
+      <c r="C93">
+        <v>27.8</v>
+      </c>
+      <c r="D93">
+        <v>332141</v>
+      </c>
+      <c r="E93">
+        <v>11.2</v>
+      </c>
+      <c r="F93">
+        <v>311</v>
+      </c>
+      <c r="G93" s="1">
+        <v>45780</v>
+      </c>
+      <c r="H93" s="1">
+        <v>45780</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383D184C-A2DB-45D2-95DE-0A26A70F4AC3}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>294568</v>
+      </c>
+      <c r="D2">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E2">
+        <v>23.22</v>
+      </c>
+      <c r="F2">
+        <v>759</v>
+      </c>
+      <c r="G2">
+        <v>13.05</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44972</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44972</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>